<commit_message>
Checkpoint commit - prawie
</commit_message>
<xml_diff>
--- a/src/egeria/pracownicy.xlsx
+++ b/src/egeria/pracownicy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
   <si>
     <t>2016-01-12</t>
   </si>
@@ -71,160 +71,202 @@
     <t>Oleg</t>
   </si>
   <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Adiunkt</t>
+  </si>
+  <si>
+    <t>II Katedra i Klinika Chirurgii Ogólnej, Gastroenterologicznej i Nowotworów Układu Pokarmowego</t>
+  </si>
+  <si>
+    <t>I Wydział Lekarski z Oddziałem Stomatologicznym</t>
+  </si>
+  <si>
+    <t>mgr</t>
+  </si>
+  <si>
+    <t>Nowak</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>Starszy referent inżynieryjno-techniczny</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Chirurgii Stomatologicznej</t>
+  </si>
+  <si>
+    <t>Bobik</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Ortopedii Szczękowej</t>
+  </si>
+  <si>
+    <t>Witold</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>Katedra i Klinika Neurologii</t>
+  </si>
+  <si>
+    <t>II Wydział Lekarski z Oddziałem Anglojęzycznym</t>
+  </si>
+  <si>
+    <t>lek. med.</t>
+  </si>
+  <si>
+    <t>Marian</t>
+  </si>
+  <si>
+    <t>Piotr</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Asystent</t>
+  </si>
+  <si>
+    <t>I Zakład Radiologii Lekarskiej</t>
+  </si>
+  <si>
+    <t>Aneta</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>II Katedra i Klinika Ginekologii</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Katedra i Klinika Otolaryngologii i Onkologii Laryngologicznej</t>
+  </si>
+  <si>
+    <t>Jakub</t>
+  </si>
+  <si>
+    <t>Jagoda</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Biologii z Genetyką</t>
+  </si>
+  <si>
+    <t>Wydział Farmaceutyczny z Oddziałem Analityki Medycznej</t>
+  </si>
+  <si>
+    <t>mgr inż.</t>
+  </si>
+  <si>
+    <t>Sylwia</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Mikrobiologii Farmaceutycznej z Pracownią Diagnostyki Mikrobiologicznej</t>
+  </si>
+  <si>
+    <t>dr n. farm.</t>
+  </si>
+  <si>
+    <t>Bartosz</t>
+  </si>
+  <si>
+    <t>Tomasz</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Farmakognozji z Pracownią Roślin Leczniczych</t>
+  </si>
+  <si>
+    <t>Michał</t>
+  </si>
+  <si>
+    <t>Magdalena</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Czesław</t>
+  </si>
+  <si>
+    <t>Iwona</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Starszy wykładowca dr</t>
+  </si>
+  <si>
+    <t>Zakład Podstaw Pielęgniarstwa i Dydaktyki Medycznej</t>
+  </si>
+  <si>
+    <t>Wydział Nauk o Zdrowiu</t>
+  </si>
+  <si>
+    <t>nieistniejący tytuł</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Asystent dr</t>
+  </si>
+  <si>
+    <t>Zakład Pielęgniarstwa Anestezjologicznego i Intensywnej Opieki Medycznej</t>
+  </si>
+  <si>
+    <t>lic.</t>
+  </si>
+  <si>
+    <t>Olan</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Specjalista inżynieryjno-techniczny</t>
+  </si>
+  <si>
+    <t>Studium Wychowania Fizycznego i Sportu</t>
+  </si>
+  <si>
     <t>12121200587</t>
-  </si>
-  <si>
-    <t>Adiunkt</t>
-  </si>
-  <si>
-    <t>II Katedra i Klinika Chirurgii Ogólnej, Gastroenterologicznej i Nowotworów Układu Pokarmowego</t>
-  </si>
-  <si>
-    <t>I Wydział Lekarski z Oddziałem Stomatologicznym</t>
-  </si>
-  <si>
-    <t>mgr</t>
-  </si>
-  <si>
-    <t>Nowak</t>
-  </si>
-  <si>
-    <t>Stefan</t>
-  </si>
-  <si>
-    <t>Starszy referent inżynieryjno-techniczny</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Chirurgii Stomatologicznej</t>
-  </si>
-  <si>
-    <t>Bobik</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Ortopedii Szczękowej</t>
-  </si>
-  <si>
-    <t>Witold</t>
-  </si>
-  <si>
-    <t>Barbara</t>
-  </si>
-  <si>
-    <t>Katedra i Klinika Neurologii</t>
-  </si>
-  <si>
-    <t>II Wydział Lekarski z Oddziałem Anglojęzycznym</t>
-  </si>
-  <si>
-    <t>lek. med.</t>
-  </si>
-  <si>
-    <t>Marian</t>
-  </si>
-  <si>
-    <t>Piotr</t>
-  </si>
-  <si>
-    <t>Asystent</t>
-  </si>
-  <si>
-    <t>I Zakład Radiologii Lekarskiej</t>
-  </si>
-  <si>
-    <t>Aneta</t>
-  </si>
-  <si>
-    <t>II Katedra i Klinika Ginekologii</t>
-  </si>
-  <si>
-    <t>Adrian</t>
-  </si>
-  <si>
-    <t>Katedra i Klinika Otolaryngologii i Onkologii Laryngologicznej</t>
-  </si>
-  <si>
-    <t>Jakub</t>
-  </si>
-  <si>
-    <t>Jagoda</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Biologii z Genetyką</t>
-  </si>
-  <si>
-    <t>Wydział Farmaceutyczny z Oddziałem Analityki Medycznej</t>
-  </si>
-  <si>
-    <t>mgr inż.</t>
-  </si>
-  <si>
-    <t>Sylwia</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Mikrobiologii Farmaceutycznej z Pracownią Diagnostyki Mikrobiologicznej</t>
-  </si>
-  <si>
-    <t>dr n. farm.</t>
-  </si>
-  <si>
-    <t>Bartosz</t>
-  </si>
-  <si>
-    <t>Tomasz</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Farmakognozji z Pracownią Roślin Leczniczych</t>
-  </si>
-  <si>
-    <t>Michał</t>
-  </si>
-  <si>
-    <t>Magdalena</t>
-  </si>
-  <si>
-    <t>Czesław</t>
-  </si>
-  <si>
-    <t>Iwona</t>
-  </si>
-  <si>
-    <t>Starszy wykładowca dr</t>
-  </si>
-  <si>
-    <t>Zakład Podstaw Pielęgniarstwa i Dydaktyki Medycznej</t>
-  </si>
-  <si>
-    <t>Wydział Nauk o Zdrowiu</t>
-  </si>
-  <si>
-    <t>nieistniejący tytuł</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Asystent dr</t>
-  </si>
-  <si>
-    <t>Zakład Pielęgniarstwa Anestezjologicznego i Intensywnej Opieki Medycznej</t>
-  </si>
-  <si>
-    <t>lic.</t>
-  </si>
-  <si>
-    <t>Olan</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>Specjalista inżynieryjno-techniczny</t>
-  </si>
-  <si>
-    <t>Studium Wychowania Fizycznego i Sportu</t>
   </si>
 </sst>
 </file>
@@ -350,7 +392,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,6 +410,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -407,20 +453,20 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:H19"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.87755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,7 +523,7 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -486,7 +532,7 @@
       <c r="G6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -503,16 +549,16 @@
       <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>14</v>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -524,21 +570,21 @@
         <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -550,22 +596,22 @@
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,25 +619,25 @@
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,19 +651,19 @@
         <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>39</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,25 +671,25 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="G12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>29</v>
+        <v>44</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,22 +700,22 @@
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>46</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,25 +723,25 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,25 +749,25 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>14</v>
+        <v>56</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,25 +775,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,22 +804,22 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>14</v>
+        <v>63</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,25 +827,25 @@
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>14</v>
+        <v>69</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>56</v>
+        <v>72</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,25 +853,25 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>14</v>
+        <v>75</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>56</v>
+        <v>78</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -847,46 +893,46 @@
   <dimension ref="A1:H547"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="A17:H19 H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.3469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.43367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8316326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -904,7 +950,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
@@ -912,7 +958,7 @@
       <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -930,15 +976,15 @@
         <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -950,21 +996,21 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -988,46 +1034,46 @@
   <dimension ref="A1:H602"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A17:H19 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.92857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1039,22 +1085,22 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,25 +1108,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,19 +1140,19 @@
         <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,25 +1160,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>29</v>
+        <v>44</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1155,46 +1201,46 @@
   <dimension ref="A1:H224"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A17:H19 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.53571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1206,22 +1252,22 @@
         <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,25 +1275,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,25 +1301,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,25 +1327,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1322,46 +1368,46 @@
   <dimension ref="A1:H245"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="A17:H19 H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.13775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.14795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1373,22 +1419,22 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,25 +1442,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>56</v>
+        <v>72</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,25 +1468,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>56</v>
+        <v>78</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Częściowo opracowane widoki do importu danych.
</commit_message>
<xml_diff>
--- a/src/egeria/pracownicy.xlsx
+++ b/src/egeria/pracownicy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="81">
   <si>
     <t>2016-01-12</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>Nowe Stanowisko</t>
   </si>
   <si>
     <t>Katedra i Zakład Biologii z Genetyką</t>
@@ -392,7 +395,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -410,10 +413,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,20 +452,20 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.87755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.3928571428572"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +522,7 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -532,7 +531,7 @@
       <c r="G6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -549,7 +548,7 @@
       <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -558,7 +557,7 @@
       <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -575,7 +574,7 @@
       <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -584,7 +583,7 @@
       <c r="G8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -601,7 +600,7 @@
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -610,7 +609,7 @@
       <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -627,7 +626,7 @@
       <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -636,7 +635,7 @@
       <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -653,7 +652,7 @@
       <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -662,7 +661,7 @@
       <c r="G11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -679,7 +678,7 @@
       <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -688,7 +687,7 @@
       <c r="G12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -705,17 +704,17 @@
       <c r="D13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="6" t="s">
         <v>49</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,25 +722,25 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="5" t="s">
         <v>52</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,25 +748,25 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="5" t="s">
         <v>57</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,25 +774,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5" t="s">
         <v>61</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,22 +803,22 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F17" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="6" t="s">
         <v>67</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,25 +826,25 @@
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="F18" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,25 +852,25 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="E19" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="F19" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -898,41 +897,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8316326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -950,7 +949,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
@@ -958,7 +957,7 @@
       <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -976,7 +975,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>22</v>
@@ -984,7 +983,7 @@
       <c r="G4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1002,7 +1001,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>22</v>
@@ -1010,7 +1009,7 @@
       <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1039,41 +1038,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1091,7 +1090,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
@@ -1099,7 +1098,7 @@
       <c r="G3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1117,7 +1116,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>37</v>
@@ -1125,7 +1124,7 @@
       <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1143,7 +1142,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -1151,7 +1150,7 @@
       <c r="G5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1169,7 +1168,7 @@
         <v>42</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>37</v>
@@ -1177,7 +1176,7 @@
       <c r="G6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1206,41 +1205,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.3928571428572"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1258,16 +1257,16 @@
         <v>46</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="6" t="s">
         <v>49</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,25 +1274,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,25 +1300,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,25 +1326,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1373,41 +1372,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.14795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.484693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1419,22 +1418,22 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="6" t="s">
         <v>67</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,25 +1441,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,25 +1467,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>67</v>
+      <c r="H5" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Import z Egerii, odsłona nr 1
</commit_message>
<xml_diff>
--- a/src/egeria/pracownicy.xlsx
+++ b/src/egeria/pracownicy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="83">
   <si>
     <t>2016-01-12</t>
   </si>
@@ -122,154 +122,160 @@
     <t>dd</t>
   </si>
   <si>
+    <t>Nowa, nieistniejąca wcześniej katedra</t>
+  </si>
+  <si>
+    <t>II Wydział Lekarski z Oddziałem Anglojęzycznym</t>
+  </si>
+  <si>
+    <t>lek. med.</t>
+  </si>
+  <si>
+    <t>Marian</t>
+  </si>
+  <si>
+    <t>Piotr</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Asystent</t>
+  </si>
+  <si>
+    <t>I Zakład Radiologii Lekarskiej</t>
+  </si>
+  <si>
+    <t>Aneta</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>II Katedra i Klinika Ginekologii</t>
+  </si>
+  <si>
+    <t>Nowy, nieistniejący wcześniej wydział</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Katedra i Klinika Otolaryngologii i Onkologii Laryngologicznej</t>
+  </si>
+  <si>
+    <t>Jakub</t>
+  </si>
+  <si>
+    <t>Jagoda</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Nowe Stanowisko</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Biologii z Genetyką</t>
+  </si>
+  <si>
+    <t>Wydział Farmaceutyczny z Oddziałem Analityki Medycznej</t>
+  </si>
+  <si>
+    <t>mgr inż.</t>
+  </si>
+  <si>
+    <t>Sylwia</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Mikrobiologii Farmaceutycznej z Pracownią Diagnostyki Mikrobiologicznej</t>
+  </si>
+  <si>
+    <t>dr n. farm.</t>
+  </si>
+  <si>
+    <t>Bartosz</t>
+  </si>
+  <si>
+    <t>Tomasz</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>Katedra i Zakład Farmakognozji z Pracownią Roślin Leczniczych</t>
+  </si>
+  <si>
+    <t>Michał</t>
+  </si>
+  <si>
+    <t>Magdalena</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Czesław</t>
+  </si>
+  <si>
+    <t>Iwona</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Starszy wykładowca dr</t>
+  </si>
+  <si>
+    <t>Zakład Podstaw Pielęgniarstwa i Dydaktyki Medycznej</t>
+  </si>
+  <si>
+    <t>Wydział Nauk o Zdrowiu</t>
+  </si>
+  <si>
+    <t>nieistniejący tytuł</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Asystent dr</t>
+  </si>
+  <si>
+    <t>Zakład Pielęgniarstwa Anestezjologicznego i Intensywnej Opieki Medycznej</t>
+  </si>
+  <si>
+    <t>lic.</t>
+  </si>
+  <si>
+    <t>Olan</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Specjalista inżynieryjno-techniczny</t>
+  </si>
+  <si>
+    <t>Studium Wychowania Fizycznego i Sportu</t>
+  </si>
+  <si>
+    <t>12121200587</t>
+  </si>
+  <si>
     <t>Katedra i Klinika Neurologii</t>
-  </si>
-  <si>
-    <t>II Wydział Lekarski z Oddziałem Anglojęzycznym</t>
-  </si>
-  <si>
-    <t>lek. med.</t>
-  </si>
-  <si>
-    <t>Marian</t>
-  </si>
-  <si>
-    <t>Piotr</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Asystent</t>
-  </si>
-  <si>
-    <t>I Zakład Radiologii Lekarskiej</t>
-  </si>
-  <si>
-    <t>Aneta</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>II Katedra i Klinika Ginekologii</t>
-  </si>
-  <si>
-    <t>Adrian</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Katedra i Klinika Otolaryngologii i Onkologii Laryngologicznej</t>
-  </si>
-  <si>
-    <t>Jakub</t>
-  </si>
-  <si>
-    <t>Jagoda</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Nowe Stanowisko</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Biologii z Genetyką</t>
-  </si>
-  <si>
-    <t>Wydział Farmaceutyczny z Oddziałem Analityki Medycznej</t>
-  </si>
-  <si>
-    <t>mgr inż.</t>
-  </si>
-  <si>
-    <t>Sylwia</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Mikrobiologii Farmaceutycznej z Pracownią Diagnostyki Mikrobiologicznej</t>
-  </si>
-  <si>
-    <t>dr n. farm.</t>
-  </si>
-  <si>
-    <t>Bartosz</t>
-  </si>
-  <si>
-    <t>Tomasz</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>Katedra i Zakład Farmakognozji z Pracownią Roślin Leczniczych</t>
-  </si>
-  <si>
-    <t>Michał</t>
-  </si>
-  <si>
-    <t>Magdalena</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>Czesław</t>
-  </si>
-  <si>
-    <t>Iwona</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>Starszy wykładowca dr</t>
-  </si>
-  <si>
-    <t>Zakład Podstaw Pielęgniarstwa i Dydaktyki Medycznej</t>
-  </si>
-  <si>
-    <t>Wydział Nauk o Zdrowiu</t>
-  </si>
-  <si>
-    <t>nieistniejący tytuł</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Asystent dr</t>
-  </si>
-  <si>
-    <t>Zakład Pielęgniarstwa Anestezjologicznego i Intensywnej Opieki Medycznej</t>
-  </si>
-  <si>
-    <t>lic.</t>
-  </si>
-  <si>
-    <t>Olan</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Specjalista inżynieryjno-techniczny</t>
-  </si>
-  <si>
-    <t>Studium Wychowania Fizycznego i Sportu</t>
-  </si>
-  <si>
-    <t>12121200587</t>
   </si>
 </sst>
 </file>
@@ -451,21 +457,21 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.3928571428572"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="55.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,7 +668,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,16 +682,16 @@
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>32</v>
@@ -699,22 +705,22 @@
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,25 +728,25 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,25 +754,25 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,25 +780,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,22 +809,22 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,25 +832,25 @@
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,25 +858,25 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -897,15 +903,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -949,7 +955,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
@@ -975,7 +981,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>22</v>
@@ -1001,7 +1007,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>22</v>
@@ -1039,14 +1045,14 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1090,13 +1096,13 @@
         <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>32</v>
@@ -1116,7 +1122,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>37</v>
@@ -1142,7 +1148,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -1165,16 +1171,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>32</v>
@@ -1205,15 +1211,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.3928571428572"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.78571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="55.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1251,22 +1257,22 @@
         <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,25 +1280,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,25 +1306,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,25 +1332,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1373,14 +1379,14 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1418,22 +1424,22 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,25 +1447,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,25 +1473,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>